<commit_message>
Updated the input configuration files and the loading functions in prevision of the integer clustered formulation
</commit_message>
<xml_diff>
--- a/ConfigFiles/ConfigIE.xlsx
+++ b/ConfigFiles/ConfigIE.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="147">
   <si>
     <t>Default value</t>
   </si>
@@ -114,6 +114,9 @@
     <t>SE</t>
   </si>
   <si>
+    <t>UK</t>
+  </si>
+  <si>
     <t>CH</t>
   </si>
   <si>
@@ -414,18 +417,6 @@
     <t>Participation to reserve markets</t>
   </si>
   <si>
-    <t>Database/FuelPrices/Coal/2015.csv</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Gas/2015.csv</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Oil/2015.csv</t>
-  </si>
-  <si>
-    <t>Database/FuelPrices/Biomass/2015.csv</t>
-  </si>
-  <si>
     <t>Price of Nuclear</t>
   </si>
   <si>
@@ -450,25 +441,22 @@
     <t>Scaled inflows</t>
   </si>
   <si>
-    <t>Simulation of the Irish power system, isolated</t>
-  </si>
-  <si>
-    <t>Database/PowerPlants/##/2015_lucy.csv</t>
+    <t>Simulation of the Irish power system, isolated.</t>
   </si>
   <si>
     <t>Simulations/simulationIE</t>
   </si>
   <si>
-    <t>GB</t>
+    <t>Database/OutageFactors/##/1h/2015.csv</t>
+  </si>
+  <si>
+    <t>Database/PowerPlants/##/2015_Lucy.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB: Ireland (IE) includes north Ireland. </t>
   </si>
   <si>
     <t>NB: UK is not considered as zone but GB is.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NB: Ireland (IE) includes north Ireland. </t>
-  </si>
-  <si>
-    <t>Database/OutageFactors/##/1h/2015.csv</t>
   </si>
 </sst>
 </file>
@@ -662,6 +650,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -956,11 +947,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="1" customWidth="1"/>
@@ -973,9 +964,9 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -985,7 +976,7 @@
       <c r="G1" s="31"/>
       <c r="H1" s="31"/>
     </row>
-    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="3" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -995,10 +986,10 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="3.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="4" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="32"/>
@@ -1007,7 +998,7 @@
       <c r="G4" s="32"/>
       <c r="H4" s="32"/>
     </row>
-    <row r="5" spans="1:8" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="9" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8"/>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1017,12 +1008,12 @@
       <c r="G5" s="19"/>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
@@ -1031,7 +1022,7 @@
       <c r="G6" s="29"/>
       <c r="H6" s="29"/>
     </row>
-    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="8.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
@@ -1040,37 +1031,37 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8"/>
       <c r="C8" s="17"/>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="10" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="11" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="12" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="13" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="14" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="15" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="16" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D18" s="14"/>
       <c r="H18" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>4</v>
@@ -1079,12 +1070,12 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>4</v>
@@ -1093,12 +1084,12 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>4</v>
@@ -1107,100 +1098,100 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="24" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="25" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="26" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="27" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="28" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="30" spans="1:8" s="9" customFormat="1" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="8"/>
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="C31" s="21">
         <v>42005</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="21">
-        <v>42014</v>
+        <v>42369</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C33" s="4">
         <v>3</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C34" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="37" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="38" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="39" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="40" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="41" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="42" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="43" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="44" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="45" spans="1:8" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="8"/>
       <c r="C45" s="17"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>4</v>
@@ -1209,42 +1200,42 @@
         <v>1</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D47" s="14"/>
       <c r="H47" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="D48" s="14"/>
       <c r="H48" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>4</v>
@@ -1254,21 +1245,21 @@
       </c>
       <c r="D49" s="14"/>
     </row>
-    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:8" s="11" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="9" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="51" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="52" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="53" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="54" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="55" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="56" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="57" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="58" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="59" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="60" spans="1:8" s="11" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="10"/>
       <c r="C60" s="18"/>
     </row>
-    <row r="61" spans="1:8" s="9" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" s="9" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="8"/>
       <c r="C61" s="17"/>
     </row>
@@ -1277,13 +1268,13 @@
         <v>2</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C62" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D62" s="23" t="s">
         <v>96</v>
-      </c>
-      <c r="D62" s="23" t="s">
-        <v>95</v>
       </c>
       <c r="H62" s="12"/>
     </row>
@@ -1292,16 +1283,16 @@
         <v>1</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>150</v>
+        <v>39</v>
+      </c>
+      <c r="C63" t="s">
+        <v>143</v>
       </c>
       <c r="D63" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H63" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,42 +1300,42 @@
         <v>3</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D64" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H64" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="C65" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C66" s="25"/>
       <c r="D66" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>0</v>
@@ -1353,64 +1344,64 @@
         <v>0.05</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H67" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D68" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H68" s="12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C69" s="25"/>
       <c r="D69" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C70" s="25"/>
       <c r="D70" s="23"/>
@@ -1423,97 +1414,89 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C71" s="25" t="s">
-        <v>132</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C71" s="25"/>
       <c r="D71" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F71" s="5">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C72" s="25" t="s">
-        <v>133</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C72" s="25"/>
       <c r="D72" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F72" s="5">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C73" s="25" t="s">
-        <v>134</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C73" s="25"/>
       <c r="D73" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F73" s="5">
-        <v>35</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C74" s="25" t="s">
-        <v>135</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C74" s="25"/>
       <c r="D74" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F74" s="5">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C75" s="25"/>
       <c r="D75" s="23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>0</v>
@@ -1524,27 +1507,27 @@
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C76" s="25"/>
       <c r="D76" s="23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" s="16" customFormat="1" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="15"/>
       <c r="C77" s="22"/>
     </row>
-    <row r="78" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:8" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="79" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="80" spans="1:8" ht="1.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="81" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="1:8" ht="9.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="83" spans="1:8" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="84" spans="1:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="85" spans="1:8" s="11" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="C85" s="18"/>
@@ -1552,13 +1535,13 @@
     <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B87" s="6"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>24</v>
@@ -1573,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -1609,7 +1592,7 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="30"/>
       <c r="B91" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C91" s="4" t="b">
         <v>0</v>
@@ -1675,7 +1658,7 @@
         <v>0</v>
       </c>
       <c r="E95" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F95" s="5" t="b">
         <v>0</v>
@@ -1780,20 +1763,20 @@
         <v>0</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="F102" s="5" t="b">
         <v>0</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="105" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="106" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="107" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="108" spans="1:8" ht="10.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="109" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="10"/>
@@ -1801,7 +1784,7 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -1809,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C112" s="5">
         <v>1</v>
@@ -1817,62 +1800,62 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C113" s="5">
         <v>1</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C114" s="5">
         <v>1</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B115" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B115" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="C115" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="118" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="119" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="120" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="121" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="122" spans="1:8" ht="3.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="123" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="124" spans="1:8" ht="1.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:8" ht="0.75" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="126" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="127" spans="1:8" ht="14.45" hidden="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="128" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="10"/>
       <c r="C128" s="18"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -1896,7 +1879,7 @@
         <v>105</v>
       </c>
       <c r="C134" s="27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,7 +1887,7 @@
         <v>106</v>
       </c>
       <c r="C135" s="27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -1920,7 +1903,7 @@
         <v>108</v>
       </c>
       <c r="C137" s="27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
@@ -1952,7 +1935,7 @@
         <v>112</v>
       </c>
       <c r="C141" s="27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -1976,7 +1959,7 @@
         <v>115</v>
       </c>
       <c r="C144" s="27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
@@ -1984,6 +1967,14 @@
         <v>116</v>
       </c>
       <c r="C145" s="27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C146" s="27" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2027,7 +2018,7 @@
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>C132:C145 C88:C102 F89:G101 F88</xm:sqref>
+          <xm:sqref>F88:G102 C88:C102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Write excel files" prompt="If set to true, one excel file per parameter will be written in the simulation environment directory.">
           <x14:formula1>
@@ -2069,7 +2060,7 @@
           <x14:formula1>
             <xm:f>[1]Lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F102:G102 G88</xm:sqref>
+          <xm:sqref>C132:C146</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2093,56 +2084,56 @@
     <col min="4" max="4" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="20" customFormat="1" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="b">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -2164,53 +2155,53 @@
     <col min="1" max="1" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="20" customFormat="1" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="20" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N1" s="20" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O1" s="20" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B2" s="26" t="b">
         <v>1</v>
@@ -2255,9 +2246,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="14.45" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B3" s="26" t="b">
         <v>1</v>
@@ -2304,7 +2295,7 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B4" s="26" t="b">
         <v>0</v>
@@ -2351,7 +2342,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B5" s="26" t="b">
         <v>0</v>
@@ -2398,7 +2389,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B6" s="26" t="b">
         <v>1</v>
@@ -2445,7 +2436,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B7" s="26" t="b">
         <v>1</v>
@@ -2492,7 +2483,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B8" s="26" t="b">
         <v>0</v>
@@ -2539,7 +2530,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B9" s="26" t="b">
         <v>0</v>
@@ -2586,7 +2577,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B10" s="26" t="b">
         <v>0</v>
@@ -2633,7 +2624,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B11" s="26" t="b">
         <v>0</v>
@@ -2680,7 +2671,7 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B12" s="26" t="b">
         <v>1</v>
@@ -2727,7 +2718,7 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B13" s="26" t="b">
         <v>1</v>
@@ -2774,7 +2765,7 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B14" s="26" t="b">
         <v>1</v>
@@ -2821,7 +2812,7 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B15" s="26" t="b">
         <v>0</v>
@@ -2868,7 +2859,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B16" s="26" t="b">
         <v>0</v>

</xml_diff>